<commit_message>
update filter related to
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase_FilterTask_Team2_Quynh.xlsx
+++ b/src/main/resources/TestCase_FilterTask_Team2_Quynh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Selenium\selenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\Selenium\selenium\FinalProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
update filter by deadline
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase_FilterTask_Team2_Quynh.xlsx
+++ b/src/main/resources/TestCase_FilterTask_Team2_Quynh.xlsx
@@ -330,12 +330,6 @@
 B6: Kiểm tra danh sách task </t>
   </si>
   <si>
-    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày lớn hơn hoặc bằng ngày hiện tại và nhỏ hơn ngày hiện tại +7.</t>
-  </si>
-  <si>
-    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày lớn hơn hoặc bằng ngày hiện tại và nhỏ hơn ngày hiện tại +15.</t>
-  </si>
-  <si>
     <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày là ngày 2/4/2024</t>
   </si>
   <si>
@@ -712,6 +706,12 @@
   </si>
   <si>
     <t>Tất cả bản ghi task có text ở cột 'Milestone' là 'Beta Release'</t>
+  </si>
+  <si>
+    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày lớn hơn ngày hiện tại và nhỏ hơn hoặc bằng ngày hiện tại +15.</t>
+  </si>
+  <si>
+    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày lớn hơn ngày hiện tại và nhỏ hơn hoặc bằng ngày hiện tại +7.</t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1157,13 +1157,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1181,10 +1181,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1203,10 +1203,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1228,7 +1228,7 @@
         <v>54</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1250,7 +1250,7 @@
         <v>55</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1272,7 +1272,7 @@
         <v>56</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1291,10 +1291,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1313,10 +1313,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1338,7 +1338,7 @@
         <v>57</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1360,7 +1360,7 @@
         <v>58</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1382,7 +1382,7 @@
         <v>59</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1401,10 +1401,10 @@
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1426,7 +1426,7 @@
         <v>60</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1448,7 +1448,7 @@
         <v>61</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1467,10 +1467,10 @@
         <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1489,10 +1489,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1511,10 +1511,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1533,10 +1533,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1558,7 +1558,7 @@
         <v>62</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1577,10 +1577,10 @@
         <v>8</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1599,7 +1599,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>64</v>
@@ -1615,16 +1615,16 @@
         <v>9</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1637,16 +1637,16 @@
         <v>9</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1709,7 +1709,7 @@
         <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>69</v>
@@ -1753,7 +1753,7 @@
         <v>8</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>71</v>
@@ -1797,7 +1797,7 @@
         <v>8</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F34" s="11" t="s">
         <v>74</v>
@@ -1819,7 +1819,7 @@
         <v>8</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>75</v>
@@ -1861,10 +1861,10 @@
         <v>8</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="148.5" x14ac:dyDescent="0.45">
@@ -1881,10 +1881,10 @@
         <v>8</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
@@ -1901,10 +1901,10 @@
         <v>8</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1921,10 +1921,10 @@
         <v>8</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1941,10 +1941,10 @@
         <v>8</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1961,10 +1961,10 @@
         <v>8</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1981,10 +1981,10 @@
         <v>8</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -2001,10 +2001,10 @@
         <v>8</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -2021,10 +2021,10 @@
         <v>8</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="148.5" x14ac:dyDescent="0.45">
@@ -2038,10 +2038,10 @@
         <v>8</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
@@ -2055,10 +2055,10 @@
         <v>8</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="148.5" x14ac:dyDescent="0.45">
@@ -2072,13 +2072,13 @@
         <v>52</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="132" x14ac:dyDescent="0.45">
@@ -2092,13 +2092,13 @@
         <v>53</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
update filter by deadline_custom
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCase_FilterTask_Team2_Quynh.xlsx
+++ b/src/main/resources/TestCase_FilterTask_Team2_Quynh.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="147">
   <si>
     <t>Test case Id</t>
   </si>
@@ -150,9 +150,6 @@
   </si>
   <si>
     <t>Kiểm tra lọc task theo 'Deadline' = 'In 15 days'</t>
-  </si>
-  <si>
-    <t>Kiểm tra lọc task theo 'Deadline' = 'Custom'</t>
   </si>
   <si>
     <t>Kiểm tra lọc task theo 'Status' = 'Todo'</t>
@@ -327,9 +324,6 @@
 B6: Kiểm tra danh sách task </t>
   </si>
   <si>
-    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày là ngày 2/4/2024</t>
-  </si>
-  <si>
     <t>Tất cả bản ghi task, ở cột status, đều chứa text là Todo</t>
   </si>
   <si>
@@ -340,15 +334,6 @@
   </si>
   <si>
     <t>Tất cả bản ghi task, ở cột status, đều chứa text là Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B1: Người dùng truy cập vào trang web rise
-B2: Đăng nhập vào hệ thống
-B3: Click vào menu Tasks
-B4: Click vào button 'Add new filter' hoặc button dấu '+'
-B5: Click vào dropdown  'Deadline' và 'Custom'
-B6: Chọn ngày 2/4/2024
-B7: Kiểm tra danh sách task </t>
   </si>
   <si>
     <t>Hiển thị thông báo lỗi: "This field is required."</t>
@@ -697,6 +682,51 @@
   </si>
   <si>
     <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày lớn hơn ngày hiện tại và nhỏ hơn hoặc bằng ngày hiện tại +7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Người dùng truy cập vào trang web rise
+B2: Đăng nhập vào hệ thống
+B3: Click vào menu Tasks
+B4: Click vào button 'Add new filter' hoặc button dấu '+'
+B5: Click vào dropdown  'Deadline' và 'Custom'
+B6: Chọn ngày (lớn hơn ngày hiện tại 3 ngày)
+B7: Kiểm tra danh sách task </t>
+  </si>
+  <si>
+    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày nhỏ hơn hoặc bằng ngày đã chọn và lớn hơn ngày hiện tại.</t>
+  </si>
+  <si>
+    <t>Kiểm tra lọc task theo 'Deadline' = 'Custom' với ngày được chọn lớn hơn ngày hiện tại</t>
+  </si>
+  <si>
+    <t>Kiểm tra lọc task theo 'Deadline' = 'Custom' với ngày được chọn bằng ngày hiện tại</t>
+  </si>
+  <si>
+    <t>Kiểm tra lọc task theo 'Deadline' = 'Custom' với ngày được chọn nhỏ hơn ngày hiện tại</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Người dùng truy cập vào trang web rise
+B2: Đăng nhập vào hệ thống
+B3: Click vào menu Tasks
+B4: Click vào button 'Add new filter' hoặc button dấu '+'
+B5: Click vào dropdown  'Deadline' và 'Custom'
+B6: Chọn ngày (nhỏ hơn ngày hiện tại 3 ngày)
+B7: Kiểm tra danh sách task </t>
+  </si>
+  <si>
+    <t>Tất cả bản ghi task, không có bản ghi nào.</t>
+  </si>
+  <si>
+    <t>Tất cả bản ghi task, ở cột deadline, đều chứa ngày bằng ngày hiện tại.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1: Người dùng truy cập vào trang web rise
+B2: Đăng nhập vào hệ thống
+B3: Click vào menu Tasks
+B4: Click vào button 'Add new filter' hoặc button dấu '+'
+B5: Click vào dropdown  'Deadline' và 'Custom'
+B6: Chọn ngày (bằng ngày hiện tại)
+B7: Kiểm tra danh sách task </t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H56"/>
+  <dimension ref="A4:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,7 +1163,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>10</v>
@@ -1142,13 +1172,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1157,7 +1187,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>11</v>
@@ -1166,10 +1196,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1179,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>12</v>
@@ -1188,10 +1218,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1201,7 +1231,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>13</v>
@@ -1210,10 +1240,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1223,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>14</v>
@@ -1232,10 +1262,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1245,7 +1275,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>15</v>
@@ -1254,10 +1284,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1267,7 +1297,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>16</v>
@@ -1276,10 +1306,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1289,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>17</v>
@@ -1298,10 +1328,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1311,7 +1341,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>18</v>
@@ -1320,10 +1350,10 @@
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1342,10 +1372,10 @@
         <v>8</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1364,10 +1394,10 @@
         <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1386,10 +1416,10 @@
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1408,10 +1438,10 @@
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1430,10 +1460,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1452,10 +1482,10 @@
         <v>8</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1474,10 +1504,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1496,10 +1526,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1518,10 +1548,10 @@
         <v>8</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1540,10 +1570,10 @@
         <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1562,10 +1592,10 @@
         <v>8</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1584,10 +1614,10 @@
         <v>8</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1600,16 +1630,16 @@
         <v>9</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1622,16 +1652,16 @@
         <v>9</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1650,10 +1680,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1672,10 +1702,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1694,10 +1724,10 @@
         <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1716,10 +1746,10 @@
         <v>8</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1738,10 +1768,10 @@
         <v>8</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -1760,10 +1790,10 @@
         <v>8</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1782,10 +1812,10 @@
         <v>8</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1804,10 +1834,10 @@
         <v>8</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -1826,10 +1856,10 @@
         <v>8</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1846,10 +1876,10 @@
         <v>8</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="148.5" x14ac:dyDescent="0.45">
@@ -1866,10 +1896,10 @@
         <v>8</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
@@ -1880,19 +1910,19 @@
         <v>9</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="132" x14ac:dyDescent="0.45">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
       <c r="A40" s="3">
         <v>36</v>
       </c>
@@ -1900,19 +1930,19 @@
         <v>9</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="132" x14ac:dyDescent="0.45">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -1920,16 +1950,16 @@
         <v>9</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1940,16 +1970,16 @@
         <v>9</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1960,16 +1990,16 @@
         <v>9</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="132" x14ac:dyDescent="0.45">
@@ -1980,39 +2010,39 @@
         <v>9</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="148.5" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="132" x14ac:dyDescent="0.45">
       <c r="A45" s="3">
         <v>41</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="132" x14ac:dyDescent="0.45">
       <c r="A46" s="3">
         <v>42</v>
       </c>
@@ -2020,16 +2050,16 @@
         <v>9</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="148.5" x14ac:dyDescent="0.45">
@@ -2037,22 +2067,22 @@
         <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D47" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="F47" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="132" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="115.5" x14ac:dyDescent="0.45">
       <c r="A48" s="3">
         <v>44</v>
       </c>
@@ -2060,41 +2090,81 @@
         <v>9</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C49" s="11"/>
-    </row>
-    <row r="50" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="C50" s="11"/>
-    </row>
-    <row r="51" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="148.5" x14ac:dyDescent="0.45">
+      <c r="A49" s="3">
+        <v>45</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="132" x14ac:dyDescent="0.45">
+      <c r="A50" s="3">
+        <v>46</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C51" s="11"/>
     </row>
-    <row r="52" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C52" s="11"/>
     </row>
-    <row r="53" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C53" s="11"/>
     </row>
-    <row r="54" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C54" s="11"/>
     </row>
-    <row r="55" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C55" s="11"/>
     </row>
-    <row r="56" spans="3:3" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
       <c r="C56" s="11"/>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C57" s="11"/>
+    </row>
+    <row r="58" spans="1:6" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="C58" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>